<commit_message>
fix: Negative Zahlen verbessert, es gibt aber noch Bugs.
</commit_message>
<xml_diff>
--- a/MA-Zeitplan.xlsx
+++ b/MA-Zeitplan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malik\OneDrive\Desktop\VSC\malik.niederhauser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DF19ACF-5829-4073-BEE1-239B312EA1E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35763907-8DD9-4E71-8EED-8B94692920A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9360" yWindow="0" windowWidth="9930" windowHeight="10170" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7270" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitplan" sheetId="1" r:id="rId1"/>
@@ -969,6 +969,18 @@
     <xf numFmtId="49" fontId="0" fillId="8" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="13" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="13" borderId="39" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="12" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1028,18 +1040,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="13" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="13" borderId="39" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="12" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1385,19 +1385,19 @@
       <c r="C4" s="19">
         <v>7</v>
       </c>
-      <c r="D4" s="58" t="s">
+      <c r="D4" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="58"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="58"/>
-      <c r="H4" s="58"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="58"/>
-      <c r="K4" s="58"/>
-      <c r="L4" s="58"/>
-      <c r="M4" s="58"/>
-      <c r="N4" s="59"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="62"/>
+      <c r="I4" s="62"/>
+      <c r="J4" s="62"/>
+      <c r="K4" s="62"/>
+      <c r="L4" s="62"/>
+      <c r="M4" s="62"/>
+      <c r="N4" s="63"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B5" s="9" t="s">
@@ -1740,27 +1740,27 @@
       <c r="N22" s="23"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B23" s="55"/>
-      <c r="C23" s="60">
+      <c r="B23" s="59"/>
+      <c r="C23" s="64">
         <v>26</v>
       </c>
-      <c r="D23" s="62" t="s">
+      <c r="D23" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="E23" s="62"/>
-      <c r="F23" s="62"/>
-      <c r="G23" s="62"/>
-      <c r="H23" s="62"/>
-      <c r="I23" s="62"/>
-      <c r="J23" s="62"/>
-      <c r="K23" s="62"/>
-      <c r="L23" s="62"/>
-      <c r="M23" s="62"/>
-      <c r="N23" s="63"/>
+      <c r="E23" s="66"/>
+      <c r="F23" s="66"/>
+      <c r="G23" s="66"/>
+      <c r="H23" s="66"/>
+      <c r="I23" s="66"/>
+      <c r="J23" s="66"/>
+      <c r="K23" s="66"/>
+      <c r="L23" s="66"/>
+      <c r="M23" s="66"/>
+      <c r="N23" s="67"/>
     </row>
     <row r="24" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="57"/>
-      <c r="C24" s="61"/>
+      <c r="B24" s="61"/>
+      <c r="C24" s="65"/>
       <c r="D24" s="17"/>
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
@@ -1793,27 +1793,27 @@
       <c r="N25" s="26"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B26" s="67"/>
-      <c r="C26" s="55">
+      <c r="B26" s="71"/>
+      <c r="C26" s="59">
         <v>28</v>
       </c>
-      <c r="D26" s="69" t="s">
+      <c r="D26" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="E26" s="69"/>
-      <c r="F26" s="69"/>
-      <c r="G26" s="69"/>
-      <c r="H26" s="69"/>
-      <c r="I26" s="69"/>
-      <c r="J26" s="69"/>
-      <c r="K26" s="69"/>
-      <c r="L26" s="69"/>
-      <c r="M26" s="69"/>
-      <c r="N26" s="70"/>
+      <c r="E26" s="73"/>
+      <c r="F26" s="73"/>
+      <c r="G26" s="73"/>
+      <c r="H26" s="73"/>
+      <c r="I26" s="73"/>
+      <c r="J26" s="73"/>
+      <c r="K26" s="73"/>
+      <c r="L26" s="73"/>
+      <c r="M26" s="73"/>
+      <c r="N26" s="74"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B27" s="68"/>
-      <c r="C27" s="57"/>
+      <c r="B27" s="72"/>
+      <c r="C27" s="61"/>
       <c r="D27" s="16"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -1894,27 +1894,27 @@
       <c r="N31" s="8"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B32" s="67"/>
-      <c r="C32" s="55">
+      <c r="B32" s="71"/>
+      <c r="C32" s="59">
         <v>33</v>
       </c>
-      <c r="D32" s="69" t="s">
+      <c r="D32" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="E32" s="69"/>
-      <c r="F32" s="69"/>
-      <c r="G32" s="69"/>
-      <c r="H32" s="69"/>
-      <c r="I32" s="69"/>
-      <c r="J32" s="69"/>
-      <c r="K32" s="69"/>
-      <c r="L32" s="69"/>
-      <c r="M32" s="69"/>
-      <c r="N32" s="70"/>
+      <c r="E32" s="73"/>
+      <c r="F32" s="73"/>
+      <c r="G32" s="73"/>
+      <c r="H32" s="73"/>
+      <c r="I32" s="73"/>
+      <c r="J32" s="73"/>
+      <c r="K32" s="73"/>
+      <c r="L32" s="73"/>
+      <c r="M32" s="73"/>
+      <c r="N32" s="74"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B33" s="68"/>
-      <c r="C33" s="57"/>
+      <c r="B33" s="72"/>
+      <c r="C33" s="61"/>
       <c r="D33" s="16"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -2021,27 +2021,27 @@
       <c r="N38" s="8"/>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B39" s="55"/>
-      <c r="C39" s="55">
+      <c r="B39" s="59"/>
+      <c r="C39" s="59">
         <v>39</v>
       </c>
-      <c r="D39" s="71" t="s">
+      <c r="D39" s="75" t="s">
         <v>24</v>
       </c>
-      <c r="E39" s="69"/>
-      <c r="F39" s="69"/>
-      <c r="G39" s="69"/>
-      <c r="H39" s="69"/>
-      <c r="I39" s="69"/>
-      <c r="J39" s="69"/>
-      <c r="K39" s="69"/>
-      <c r="L39" s="69"/>
-      <c r="M39" s="69"/>
-      <c r="N39" s="70"/>
+      <c r="E39" s="73"/>
+      <c r="F39" s="73"/>
+      <c r="G39" s="73"/>
+      <c r="H39" s="73"/>
+      <c r="I39" s="73"/>
+      <c r="J39" s="73"/>
+      <c r="K39" s="73"/>
+      <c r="L39" s="73"/>
+      <c r="M39" s="73"/>
+      <c r="N39" s="74"/>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B40" s="57"/>
-      <c r="C40" s="57"/>
+      <c r="B40" s="61"/>
+      <c r="C40" s="61"/>
       <c r="D40" s="16"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -2089,27 +2089,27 @@
       <c r="N42" s="8"/>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B43" s="55"/>
-      <c r="C43" s="66">
+      <c r="B43" s="59"/>
+      <c r="C43" s="70">
         <v>42</v>
       </c>
-      <c r="D43" s="64" t="s">
+      <c r="D43" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="E43" s="64"/>
-      <c r="F43" s="64"/>
-      <c r="G43" s="64"/>
-      <c r="H43" s="64"/>
-      <c r="I43" s="64"/>
-      <c r="J43" s="64"/>
-      <c r="K43" s="64"/>
-      <c r="L43" s="64"/>
-      <c r="M43" s="64"/>
-      <c r="N43" s="65"/>
+      <c r="E43" s="68"/>
+      <c r="F43" s="68"/>
+      <c r="G43" s="68"/>
+      <c r="H43" s="68"/>
+      <c r="I43" s="68"/>
+      <c r="J43" s="68"/>
+      <c r="K43" s="68"/>
+      <c r="L43" s="68"/>
+      <c r="M43" s="68"/>
+      <c r="N43" s="69"/>
     </row>
     <row r="44" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B44" s="56"/>
-      <c r="C44" s="61"/>
+      <c r="B44" s="60"/>
+      <c r="C44" s="65"/>
       <c r="D44" s="17"/>
       <c r="E44" s="12"/>
       <c r="F44" s="12"/>
@@ -2150,7 +2150,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18EAA04E-3179-4EA5-8781-1F5ACEA7B7D4}">
   <dimension ref="D5:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E4" zoomScale="75" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E5" zoomScale="75" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -2198,17 +2198,17 @@
       </c>
     </row>
     <row r="7" spans="4:12" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D7" s="72" t="s">
+      <c r="D7" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="73"/>
-      <c r="F7" s="73"/>
-      <c r="G7" s="73"/>
-      <c r="H7" s="73"/>
-      <c r="I7" s="73"/>
-      <c r="J7" s="73"/>
-      <c r="K7" s="73"/>
-      <c r="L7" s="74"/>
+      <c r="E7" s="77"/>
+      <c r="F7" s="77"/>
+      <c r="G7" s="77"/>
+      <c r="H7" s="77"/>
+      <c r="I7" s="77"/>
+      <c r="J7" s="77"/>
+      <c r="K7" s="77"/>
+      <c r="L7" s="78"/>
     </row>
     <row r="8" spans="4:12" ht="80" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D8" s="41"/>
@@ -2225,28 +2225,28 @@
       <c r="I8" s="29"/>
       <c r="J8" s="30"/>
       <c r="K8" s="31"/>
-      <c r="L8" s="78" t="s">
+      <c r="L8" s="58" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="9" spans="4:12" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D9" s="72" t="s">
+      <c r="D9" s="76" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
-      <c r="G9" s="73"/>
-      <c r="H9" s="73"/>
-      <c r="I9" s="73"/>
-      <c r="J9" s="73"/>
-      <c r="K9" s="73"/>
-      <c r="L9" s="74"/>
+      <c r="E9" s="77"/>
+      <c r="F9" s="77"/>
+      <c r="G9" s="77"/>
+      <c r="H9" s="77"/>
+      <c r="I9" s="77"/>
+      <c r="J9" s="77"/>
+      <c r="K9" s="77"/>
+      <c r="L9" s="78"/>
     </row>
     <row r="10" spans="4:12" ht="80" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D10" s="75" t="s">
+      <c r="D10" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="76" t="s">
+      <c r="E10" s="56" t="s">
         <v>46</v>
       </c>
       <c r="F10" s="49" t="s">
@@ -2262,20 +2262,20 @@
       <c r="L10" s="42"/>
     </row>
     <row r="11" spans="4:12" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D11" s="72" t="s">
+      <c r="D11" s="76" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="73"/>
-      <c r="F11" s="73"/>
-      <c r="G11" s="73"/>
-      <c r="H11" s="73"/>
-      <c r="I11" s="73"/>
-      <c r="J11" s="73"/>
-      <c r="K11" s="73"/>
-      <c r="L11" s="74"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="77"/>
+      <c r="G11" s="77"/>
+      <c r="H11" s="77"/>
+      <c r="I11" s="77"/>
+      <c r="J11" s="77"/>
+      <c r="K11" s="77"/>
+      <c r="L11" s="78"/>
     </row>
     <row r="12" spans="4:12" ht="80" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D12" s="77" t="s">
+      <c r="D12" s="57" t="s">
         <v>47</v>
       </c>
       <c r="E12" s="51" t="s">

</xml_diff>

<commit_message>
feat: Display hinzugefügt (noch nicht verknüpft).
</commit_message>
<xml_diff>
--- a/MA-Zeitplan.xlsx
+++ b/MA-Zeitplan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malik\OneDrive\Desktop\VSC\malik.niederhauser\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/30322ea3847d01b2/Desktop/VSC/malik.niederhauser/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35763907-8DD9-4E71-8EED-8B94692920A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{35763907-8DD9-4E71-8EED-8B94692920A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B88CD22-EC21-49A0-AE21-D46FE17DFAFE}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7270" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitplan" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="53">
   <si>
     <t>KW</t>
   </si>
@@ -202,6 +202,19 @@
 - Negative Zahlen bearbeitbar machen
 - Assembler updaten
 - Display machen und mit RAM verknüpfen</t>
+  </si>
+  <si>
+    <t>- Display und CPU bzw. RAM verknüpfen
+- Display optimieren</t>
+  </si>
+  <si>
+    <t>- Display mit CPU verknüpfen
+- Display Optimisation beginnen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Beide Ziele umgesetzt
+- Display herumprobiert
+- </t>
   </si>
 </sst>
 </file>
@@ -888,9 +901,6 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -936,9 +946,6 @@
     <xf numFmtId="49" fontId="0" fillId="7" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="9" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1040,6 +1047,12 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="20" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1385,19 +1398,19 @@
       <c r="C4" s="19">
         <v>7</v>
       </c>
-      <c r="D4" s="62" t="s">
+      <c r="D4" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="62"/>
-      <c r="I4" s="62"/>
-      <c r="J4" s="62"/>
-      <c r="K4" s="62"/>
-      <c r="L4" s="62"/>
-      <c r="M4" s="62"/>
-      <c r="N4" s="63"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="60"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="60"/>
+      <c r="M4" s="60"/>
+      <c r="N4" s="61"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B5" s="9" t="s">
@@ -1740,27 +1753,27 @@
       <c r="N22" s="23"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B23" s="59"/>
-      <c r="C23" s="64">
+      <c r="B23" s="57"/>
+      <c r="C23" s="62">
         <v>26</v>
       </c>
-      <c r="D23" s="66" t="s">
+      <c r="D23" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="E23" s="66"/>
-      <c r="F23" s="66"/>
-      <c r="G23" s="66"/>
-      <c r="H23" s="66"/>
-      <c r="I23" s="66"/>
-      <c r="J23" s="66"/>
-      <c r="K23" s="66"/>
-      <c r="L23" s="66"/>
-      <c r="M23" s="66"/>
-      <c r="N23" s="67"/>
+      <c r="E23" s="64"/>
+      <c r="F23" s="64"/>
+      <c r="G23" s="64"/>
+      <c r="H23" s="64"/>
+      <c r="I23" s="64"/>
+      <c r="J23" s="64"/>
+      <c r="K23" s="64"/>
+      <c r="L23" s="64"/>
+      <c r="M23" s="64"/>
+      <c r="N23" s="65"/>
     </row>
     <row r="24" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="61"/>
-      <c r="C24" s="65"/>
+      <c r="B24" s="59"/>
+      <c r="C24" s="63"/>
       <c r="D24" s="17"/>
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
@@ -1793,27 +1806,27 @@
       <c r="N25" s="26"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B26" s="71"/>
-      <c r="C26" s="59">
+      <c r="B26" s="69"/>
+      <c r="C26" s="57">
         <v>28</v>
       </c>
-      <c r="D26" s="73" t="s">
+      <c r="D26" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="E26" s="73"/>
-      <c r="F26" s="73"/>
-      <c r="G26" s="73"/>
-      <c r="H26" s="73"/>
-      <c r="I26" s="73"/>
-      <c r="J26" s="73"/>
-      <c r="K26" s="73"/>
-      <c r="L26" s="73"/>
-      <c r="M26" s="73"/>
-      <c r="N26" s="74"/>
+      <c r="E26" s="71"/>
+      <c r="F26" s="71"/>
+      <c r="G26" s="71"/>
+      <c r="H26" s="71"/>
+      <c r="I26" s="71"/>
+      <c r="J26" s="71"/>
+      <c r="K26" s="71"/>
+      <c r="L26" s="71"/>
+      <c r="M26" s="71"/>
+      <c r="N26" s="72"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B27" s="72"/>
-      <c r="C27" s="61"/>
+      <c r="B27" s="70"/>
+      <c r="C27" s="59"/>
       <c r="D27" s="16"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -1894,27 +1907,27 @@
       <c r="N31" s="8"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B32" s="71"/>
-      <c r="C32" s="59">
+      <c r="B32" s="69"/>
+      <c r="C32" s="57">
         <v>33</v>
       </c>
-      <c r="D32" s="73" t="s">
+      <c r="D32" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="E32" s="73"/>
-      <c r="F32" s="73"/>
-      <c r="G32" s="73"/>
-      <c r="H32" s="73"/>
-      <c r="I32" s="73"/>
-      <c r="J32" s="73"/>
-      <c r="K32" s="73"/>
-      <c r="L32" s="73"/>
-      <c r="M32" s="73"/>
-      <c r="N32" s="74"/>
+      <c r="E32" s="71"/>
+      <c r="F32" s="71"/>
+      <c r="G32" s="71"/>
+      <c r="H32" s="71"/>
+      <c r="I32" s="71"/>
+      <c r="J32" s="71"/>
+      <c r="K32" s="71"/>
+      <c r="L32" s="71"/>
+      <c r="M32" s="71"/>
+      <c r="N32" s="72"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B33" s="72"/>
-      <c r="C33" s="61"/>
+      <c r="B33" s="70"/>
+      <c r="C33" s="59"/>
       <c r="D33" s="16"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -2021,27 +2034,27 @@
       <c r="N38" s="8"/>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B39" s="59"/>
-      <c r="C39" s="59">
+      <c r="B39" s="57"/>
+      <c r="C39" s="57">
         <v>39</v>
       </c>
-      <c r="D39" s="75" t="s">
+      <c r="D39" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="E39" s="73"/>
-      <c r="F39" s="73"/>
-      <c r="G39" s="73"/>
-      <c r="H39" s="73"/>
-      <c r="I39" s="73"/>
-      <c r="J39" s="73"/>
-      <c r="K39" s="73"/>
-      <c r="L39" s="73"/>
-      <c r="M39" s="73"/>
-      <c r="N39" s="74"/>
+      <c r="E39" s="71"/>
+      <c r="F39" s="71"/>
+      <c r="G39" s="71"/>
+      <c r="H39" s="71"/>
+      <c r="I39" s="71"/>
+      <c r="J39" s="71"/>
+      <c r="K39" s="71"/>
+      <c r="L39" s="71"/>
+      <c r="M39" s="71"/>
+      <c r="N39" s="72"/>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B40" s="61"/>
-      <c r="C40" s="61"/>
+      <c r="B40" s="59"/>
+      <c r="C40" s="59"/>
       <c r="D40" s="16"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -2089,27 +2102,27 @@
       <c r="N42" s="8"/>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B43" s="59"/>
-      <c r="C43" s="70">
+      <c r="B43" s="57"/>
+      <c r="C43" s="68">
         <v>42</v>
       </c>
-      <c r="D43" s="68" t="s">
+      <c r="D43" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="E43" s="68"/>
-      <c r="F43" s="68"/>
-      <c r="G43" s="68"/>
-      <c r="H43" s="68"/>
-      <c r="I43" s="68"/>
-      <c r="J43" s="68"/>
-      <c r="K43" s="68"/>
-      <c r="L43" s="68"/>
-      <c r="M43" s="68"/>
-      <c r="N43" s="69"/>
+      <c r="E43" s="66"/>
+      <c r="F43" s="66"/>
+      <c r="G43" s="66"/>
+      <c r="H43" s="66"/>
+      <c r="I43" s="66"/>
+      <c r="J43" s="66"/>
+      <c r="K43" s="66"/>
+      <c r="L43" s="66"/>
+      <c r="M43" s="66"/>
+      <c r="N43" s="67"/>
     </row>
     <row r="44" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B44" s="60"/>
-      <c r="C44" s="65"/>
+      <c r="B44" s="58"/>
+      <c r="C44" s="63"/>
       <c r="D44" s="17"/>
       <c r="E44" s="12"/>
       <c r="F44" s="12"/>
@@ -2161,7 +2174,7 @@
     <col min="6" max="6" width="40.36328125" customWidth="1"/>
     <col min="7" max="7" width="38.1796875" customWidth="1"/>
     <col min="8" max="8" width="36.26953125" customWidth="1"/>
-    <col min="9" max="9" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.90625" customWidth="1"/>
     <col min="10" max="10" width="6.7265625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.90625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="32.6328125" customWidth="1"/>
@@ -2169,129 +2182,135 @@
   <sheetData>
     <row r="5" spans="4:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="6" spans="4:12" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="33" t="s">
+      <c r="E6" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="34" t="s">
+      <c r="F6" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="35" t="s">
+      <c r="G6" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="36" t="s">
+      <c r="H6" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="37" t="s">
+      <c r="I6" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="38" t="s">
+      <c r="J6" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="K6" s="39" t="s">
+      <c r="K6" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="L6" s="40" t="s">
+      <c r="L6" s="39" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="4:12" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D7" s="76" t="s">
+      <c r="D7" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="77"/>
-      <c r="F7" s="77"/>
-      <c r="G7" s="77"/>
-      <c r="H7" s="77"/>
-      <c r="I7" s="77"/>
-      <c r="J7" s="77"/>
-      <c r="K7" s="77"/>
-      <c r="L7" s="78"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="75"/>
+      <c r="G7" s="75"/>
+      <c r="H7" s="75"/>
+      <c r="I7" s="75"/>
+      <c r="J7" s="75"/>
+      <c r="K7" s="75"/>
+      <c r="L7" s="76"/>
     </row>
     <row r="8" spans="4:12" ht="80" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D8" s="41"/>
+      <c r="D8" s="40"/>
       <c r="E8" s="27"/>
-      <c r="F8" s="52" t="s">
+      <c r="F8" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="43" t="s">
+      <c r="G8" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="H8" s="54" t="s">
+      <c r="H8" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="I8" s="29"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="58" t="s">
+      <c r="I8" s="78" t="s">
+        <v>51</v>
+      </c>
+      <c r="J8" s="29"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="56" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="9" spans="4:12" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D9" s="76" t="s">
+      <c r="D9" s="74" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="77"/>
-      <c r="F9" s="77"/>
-      <c r="G9" s="77"/>
-      <c r="H9" s="77"/>
-      <c r="I9" s="77"/>
-      <c r="J9" s="77"/>
-      <c r="K9" s="77"/>
-      <c r="L9" s="78"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="75"/>
+      <c r="G9" s="75"/>
+      <c r="H9" s="75"/>
+      <c r="I9" s="75"/>
+      <c r="J9" s="75"/>
+      <c r="K9" s="75"/>
+      <c r="L9" s="76"/>
     </row>
     <row r="10" spans="4:12" ht="80" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D10" s="55" t="s">
+      <c r="D10" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="56" t="s">
+      <c r="E10" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="F10" s="49" t="s">
+      <c r="F10" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="G10" s="43" t="s">
+      <c r="G10" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="28"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="31"/>
-      <c r="L10" s="42"/>
+      <c r="H10" s="52" t="s">
+        <v>52</v>
+      </c>
+      <c r="I10" s="28"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="41"/>
     </row>
     <row r="11" spans="4:12" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D11" s="76" t="s">
+      <c r="D11" s="74" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="77"/>
-      <c r="F11" s="77"/>
-      <c r="G11" s="77"/>
-      <c r="H11" s="77"/>
-      <c r="I11" s="77"/>
-      <c r="J11" s="77"/>
-      <c r="K11" s="77"/>
-      <c r="L11" s="78"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="75"/>
+      <c r="G11" s="75"/>
+      <c r="H11" s="75"/>
+      <c r="I11" s="75"/>
+      <c r="J11" s="75"/>
+      <c r="K11" s="75"/>
+      <c r="L11" s="76"/>
     </row>
     <row r="12" spans="4:12" ht="80" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D12" s="57" t="s">
+      <c r="D12" s="55" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="51" t="s">
+      <c r="E12" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="F12" s="53" t="s">
+      <c r="F12" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="G12" s="50" t="s">
+      <c r="G12" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="H12" s="44"/>
-      <c r="I12" s="45"/>
-      <c r="J12" s="46"/>
-      <c r="K12" s="47"/>
-      <c r="L12" s="48"/>
+      <c r="H12" s="77" t="s">
+        <v>50</v>
+      </c>
+      <c r="I12" s="43"/>
+      <c r="J12" s="44"/>
+      <c r="K12" s="45"/>
+      <c r="L12" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
fix: GUI updated, funktioniert aber in main.py noch nicht.
</commit_message>
<xml_diff>
--- a/MA-Zeitplan.xlsx
+++ b/MA-Zeitplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/30322ea3847d01b2/Desktop/VSC/malik.niederhauser/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{35763907-8DD9-4E71-8EED-8B94692920A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B88CD22-EC21-49A0-AE21-D46FE17DFAFE}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{35763907-8DD9-4E71-8EED-8B94692920A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62B12800-7A9D-4B54-A446-2A30F9660DE8}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="54">
   <si>
     <t>KW</t>
   </si>
@@ -215,6 +215,9 @@
     <t xml:space="preserve">- Beide Ziele umgesetzt
 - Display herumprobiert
 - </t>
+  </si>
+  <si>
+    <t>- Code strukturieren für besseren Überblick</t>
   </si>
 </sst>
 </file>
@@ -946,9 +949,6 @@
     <xf numFmtId="49" fontId="0" fillId="7" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="10" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -988,6 +988,12 @@
     <xf numFmtId="49" fontId="0" fillId="12" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="20" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1048,11 +1054,8 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="20" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="20" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1398,19 +1401,19 @@
       <c r="C4" s="19">
         <v>7</v>
       </c>
-      <c r="D4" s="60" t="s">
+      <c r="D4" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60"/>
-      <c r="M4" s="60"/>
-      <c r="N4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="61"/>
+      <c r="M4" s="61"/>
+      <c r="N4" s="62"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B5" s="9" t="s">
@@ -1753,27 +1756,27 @@
       <c r="N22" s="23"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B23" s="57"/>
-      <c r="C23" s="62">
+      <c r="B23" s="58"/>
+      <c r="C23" s="63">
         <v>26</v>
       </c>
-      <c r="D23" s="64" t="s">
+      <c r="D23" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="E23" s="64"/>
-      <c r="F23" s="64"/>
-      <c r="G23" s="64"/>
-      <c r="H23" s="64"/>
-      <c r="I23" s="64"/>
-      <c r="J23" s="64"/>
-      <c r="K23" s="64"/>
-      <c r="L23" s="64"/>
-      <c r="M23" s="64"/>
-      <c r="N23" s="65"/>
+      <c r="E23" s="65"/>
+      <c r="F23" s="65"/>
+      <c r="G23" s="65"/>
+      <c r="H23" s="65"/>
+      <c r="I23" s="65"/>
+      <c r="J23" s="65"/>
+      <c r="K23" s="65"/>
+      <c r="L23" s="65"/>
+      <c r="M23" s="65"/>
+      <c r="N23" s="66"/>
     </row>
     <row r="24" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="59"/>
-      <c r="C24" s="63"/>
+      <c r="B24" s="60"/>
+      <c r="C24" s="64"/>
       <c r="D24" s="17"/>
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
@@ -1806,27 +1809,27 @@
       <c r="N25" s="26"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B26" s="69"/>
-      <c r="C26" s="57">
+      <c r="B26" s="70"/>
+      <c r="C26" s="58">
         <v>28</v>
       </c>
-      <c r="D26" s="71" t="s">
+      <c r="D26" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="E26" s="71"/>
-      <c r="F26" s="71"/>
-      <c r="G26" s="71"/>
-      <c r="H26" s="71"/>
-      <c r="I26" s="71"/>
-      <c r="J26" s="71"/>
-      <c r="K26" s="71"/>
-      <c r="L26" s="71"/>
-      <c r="M26" s="71"/>
-      <c r="N26" s="72"/>
+      <c r="E26" s="72"/>
+      <c r="F26" s="72"/>
+      <c r="G26" s="72"/>
+      <c r="H26" s="72"/>
+      <c r="I26" s="72"/>
+      <c r="J26" s="72"/>
+      <c r="K26" s="72"/>
+      <c r="L26" s="72"/>
+      <c r="M26" s="72"/>
+      <c r="N26" s="73"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B27" s="70"/>
-      <c r="C27" s="59"/>
+      <c r="B27" s="71"/>
+      <c r="C27" s="60"/>
       <c r="D27" s="16"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -1907,27 +1910,27 @@
       <c r="N31" s="8"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B32" s="69"/>
-      <c r="C32" s="57">
+      <c r="B32" s="70"/>
+      <c r="C32" s="58">
         <v>33</v>
       </c>
-      <c r="D32" s="71" t="s">
+      <c r="D32" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="E32" s="71"/>
-      <c r="F32" s="71"/>
-      <c r="G32" s="71"/>
-      <c r="H32" s="71"/>
-      <c r="I32" s="71"/>
-      <c r="J32" s="71"/>
-      <c r="K32" s="71"/>
-      <c r="L32" s="71"/>
-      <c r="M32" s="71"/>
-      <c r="N32" s="72"/>
+      <c r="E32" s="72"/>
+      <c r="F32" s="72"/>
+      <c r="G32" s="72"/>
+      <c r="H32" s="72"/>
+      <c r="I32" s="72"/>
+      <c r="J32" s="72"/>
+      <c r="K32" s="72"/>
+      <c r="L32" s="72"/>
+      <c r="M32" s="72"/>
+      <c r="N32" s="73"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B33" s="70"/>
-      <c r="C33" s="59"/>
+      <c r="B33" s="71"/>
+      <c r="C33" s="60"/>
       <c r="D33" s="16"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -2034,27 +2037,27 @@
       <c r="N38" s="8"/>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B39" s="57"/>
-      <c r="C39" s="57">
+      <c r="B39" s="58"/>
+      <c r="C39" s="58">
         <v>39</v>
       </c>
-      <c r="D39" s="73" t="s">
+      <c r="D39" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="E39" s="71"/>
-      <c r="F39" s="71"/>
-      <c r="G39" s="71"/>
-      <c r="H39" s="71"/>
-      <c r="I39" s="71"/>
-      <c r="J39" s="71"/>
-      <c r="K39" s="71"/>
-      <c r="L39" s="71"/>
-      <c r="M39" s="71"/>
-      <c r="N39" s="72"/>
+      <c r="E39" s="72"/>
+      <c r="F39" s="72"/>
+      <c r="G39" s="72"/>
+      <c r="H39" s="72"/>
+      <c r="I39" s="72"/>
+      <c r="J39" s="72"/>
+      <c r="K39" s="72"/>
+      <c r="L39" s="72"/>
+      <c r="M39" s="72"/>
+      <c r="N39" s="73"/>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B40" s="59"/>
-      <c r="C40" s="59"/>
+      <c r="B40" s="60"/>
+      <c r="C40" s="60"/>
       <c r="D40" s="16"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -2102,27 +2105,27 @@
       <c r="N42" s="8"/>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B43" s="57"/>
-      <c r="C43" s="68">
+      <c r="B43" s="58"/>
+      <c r="C43" s="69">
         <v>42</v>
       </c>
-      <c r="D43" s="66" t="s">
+      <c r="D43" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="E43" s="66"/>
-      <c r="F43" s="66"/>
-      <c r="G43" s="66"/>
-      <c r="H43" s="66"/>
-      <c r="I43" s="66"/>
-      <c r="J43" s="66"/>
-      <c r="K43" s="66"/>
-      <c r="L43" s="66"/>
-      <c r="M43" s="66"/>
-      <c r="N43" s="67"/>
+      <c r="E43" s="67"/>
+      <c r="F43" s="67"/>
+      <c r="G43" s="67"/>
+      <c r="H43" s="67"/>
+      <c r="I43" s="67"/>
+      <c r="J43" s="67"/>
+      <c r="K43" s="67"/>
+      <c r="L43" s="67"/>
+      <c r="M43" s="67"/>
+      <c r="N43" s="68"/>
     </row>
     <row r="44" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B44" s="58"/>
-      <c r="C44" s="63"/>
+      <c r="B44" s="59"/>
+      <c r="C44" s="64"/>
       <c r="D44" s="17"/>
       <c r="E44" s="12"/>
       <c r="F44" s="12"/>
@@ -2163,8 +2166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18EAA04E-3179-4EA5-8781-1F5ACEA7B7D4}">
   <dimension ref="D5:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E5" zoomScale="75" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2174,7 +2177,7 @@
     <col min="6" max="6" width="40.36328125" customWidth="1"/>
     <col min="7" max="7" width="38.1796875" customWidth="1"/>
     <col min="8" max="8" width="36.26953125" customWidth="1"/>
-    <col min="9" max="9" width="31.90625" customWidth="1"/>
+    <col min="9" max="9" width="40.54296875" customWidth="1"/>
     <col min="10" max="10" width="6.7265625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.90625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="32.6328125" customWidth="1"/>
@@ -2211,66 +2214,66 @@
       </c>
     </row>
     <row r="7" spans="4:12" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D7" s="74" t="s">
+      <c r="D7" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="75"/>
-      <c r="F7" s="75"/>
-      <c r="G7" s="75"/>
-      <c r="H7" s="75"/>
-      <c r="I7" s="75"/>
-      <c r="J7" s="75"/>
-      <c r="K7" s="75"/>
-      <c r="L7" s="76"/>
+      <c r="E7" s="76"/>
+      <c r="F7" s="76"/>
+      <c r="G7" s="76"/>
+      <c r="H7" s="76"/>
+      <c r="I7" s="76"/>
+      <c r="J7" s="76"/>
+      <c r="K7" s="76"/>
+      <c r="L7" s="77"/>
     </row>
     <row r="8" spans="4:12" ht="80" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D8" s="40"/>
       <c r="E8" s="27"/>
-      <c r="F8" s="50" t="s">
+      <c r="F8" s="49" t="s">
         <v>42</v>
       </c>
       <c r="G8" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="H8" s="52" t="s">
+      <c r="H8" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="I8" s="78" t="s">
+      <c r="I8" s="57" t="s">
         <v>51</v>
       </c>
       <c r="J8" s="29"/>
       <c r="K8" s="30"/>
-      <c r="L8" s="56" t="s">
+      <c r="L8" s="55" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="9" spans="4:12" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D9" s="74" t="s">
+      <c r="D9" s="75" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="75"/>
-      <c r="F9" s="75"/>
-      <c r="G9" s="75"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="75"/>
-      <c r="J9" s="75"/>
-      <c r="K9" s="75"/>
-      <c r="L9" s="76"/>
+      <c r="E9" s="76"/>
+      <c r="F9" s="76"/>
+      <c r="G9" s="76"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="76"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="76"/>
+      <c r="L9" s="77"/>
     </row>
     <row r="10" spans="4:12" ht="80" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D10" s="53" t="s">
+      <c r="D10" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="54" t="s">
+      <c r="E10" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="F10" s="47" t="s">
+      <c r="F10" s="46" t="s">
         <v>40</v>
       </c>
       <c r="G10" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="52" t="s">
+      <c r="H10" s="51" t="s">
         <v>52</v>
       </c>
       <c r="I10" s="28"/>
@@ -2279,38 +2282,40 @@
       <c r="L10" s="41"/>
     </row>
     <row r="11" spans="4:12" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D11" s="74" t="s">
+      <c r="D11" s="75" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="75"/>
-      <c r="F11" s="75"/>
-      <c r="G11" s="75"/>
-      <c r="H11" s="75"/>
-      <c r="I11" s="75"/>
-      <c r="J11" s="75"/>
-      <c r="K11" s="75"/>
-      <c r="L11" s="76"/>
+      <c r="E11" s="76"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="76"/>
+      <c r="H11" s="76"/>
+      <c r="I11" s="76"/>
+      <c r="J11" s="76"/>
+      <c r="K11" s="76"/>
+      <c r="L11" s="77"/>
     </row>
     <row r="12" spans="4:12" ht="80" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D12" s="55" t="s">
+      <c r="D12" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="49" t="s">
+      <c r="E12" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="F12" s="51" t="s">
+      <c r="F12" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="G12" s="48" t="s">
+      <c r="G12" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="H12" s="77" t="s">
+      <c r="H12" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="I12" s="43"/>
-      <c r="J12" s="44"/>
-      <c r="K12" s="45"/>
-      <c r="L12" s="46"/>
+      <c r="I12" s="78" t="s">
+        <v>53</v>
+      </c>
+      <c r="J12" s="43"/>
+      <c r="K12" s="44"/>
+      <c r="L12" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>